<commit_message>
Mold Man app, v0.2 commit
</commit_message>
<xml_diff>
--- a/excelapp1/sample.xlsx
+++ b/excelapp1/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyWorks\mold_man\excelapp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59CA195-E567-48B5-96BF-DD35B06FA9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35912C6-7557-47CE-BFC6-480BA05D0F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22620" yWindow="5325" windowWidth="23100" windowHeight="10155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="13" r:id="rId1"/>
@@ -34,6 +34,128 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+  <si>
+    <t>管理籍</t>
+  </si>
+  <si>
+    <t>製品名</t>
+  </si>
+  <si>
+    <t>中型</t>
+  </si>
+  <si>
+    <t>外寸長</t>
+  </si>
+  <si>
+    <t>外寸幅</t>
+  </si>
+  <si>
+    <t>外寸高</t>
+  </si>
+  <si>
+    <t>内寸長</t>
+  </si>
+  <si>
+    <t>内寸幅</t>
+  </si>
+  <si>
+    <t>内寸深</t>
+  </si>
+  <si>
+    <t>蓋</t>
+  </si>
+  <si>
+    <t>蓋付</t>
+  </si>
+  <si>
+    <t>製造年月</t>
+  </si>
+  <si>
+    <t>用途</t>
+  </si>
+  <si>
+    <t>管理籍　：</t>
+    <rPh sb="0" eb="3">
+      <t>カンリセキ</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>外寸（長さ）：</t>
+    <rPh sb="0" eb="2">
+      <t>ガイスン</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ナガ</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>外寸（幅）：</t>
+    <rPh sb="0" eb="2">
+      <t>ガイスン</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ハバ</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>外寸（高さ）：</t>
+    <rPh sb="0" eb="2">
+      <t>ガイスン</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>タカ</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>内寸（長さ）：</t>
+    <rPh sb="0" eb="2">
+      <t>ナイスン</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ナガ</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>内寸（幅）：</t>
+    <rPh sb="0" eb="2">
+      <t>ナイスン</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ハバ</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>内寸（高さ）：</t>
+    <rPh sb="0" eb="2">
+      <t>ナイスン</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>タカ</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>製品名：</t>
+    <rPh sb="0" eb="3">
+      <t>セイヒンメイ</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>～</t>
+    <phoneticPr fontId="10"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
@@ -109,15 +231,21 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -156,6 +284,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -188,8 +331,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Header1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -572,14 +717,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C179F2-DC22-4382-91F2-D8A249DF793B}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="10"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
MoldMan app. v0.22a r2 commit
</commit_message>
<xml_diff>
--- a/excelapp1/sample.xlsx
+++ b/excelapp1/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyWorks\mold_man\excelapp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35912C6-7557-47CE-BFC6-480BA05D0F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FCE9BA-D870-4485-87B2-ABD13B29E273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22620" yWindow="5325" windowWidth="23100" windowHeight="10155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25020" yWindow="5445" windowWidth="16440" windowHeight="10155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="13" r:id="rId1"/>
@@ -158,11 +158,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="176" formatCode="#,##0.0&quot;人月&quot;"/>
+    <numFmt numFmtId="178" formatCode="yyyy/m"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="10.4"/>
       <name val="ＭＳ 明朝"/>
@@ -228,6 +229,19 @@
       <sz val="6"/>
       <name val="ＭＳ 明朝"/>
       <family val="1"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -240,7 +254,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,10 +345,14 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="178" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Header1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -720,112 +738,118 @@
   <dimension ref="A2:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="11" width="9.140625" style="2"/>
+    <col min="12" max="12" width="9.140625" style="4"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:13">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="D3" t="s">
+      <c r="B3" s="1"/>
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="I3" t="s">
+      <c r="G3" s="1"/>
+      <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="D4" t="s">
+      <c r="B4" s="1"/>
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="I4" t="s">
+      <c r="G4" s="1"/>
+      <c r="I4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="D5" t="s">
+      <c r="B5" s="1"/>
+      <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="I5" t="s">
+      <c r="G5" s="1"/>
+      <c r="I5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="10"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>